<commit_message>
added planetscale benchmark results
</commit_message>
<xml_diff>
--- a/2023/ycsb/mysql_mariadb/aggregation.xlsx
+++ b/2023/ycsb/mysql_mariadb/aggregation.xlsx
@@ -116,9 +116,9 @@
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="2224908713385522181" xfId="1" hidden="0"/>
-    <cellStyle name="-7304385740909460175" xfId="2" hidden="0"/>
-    <cellStyle name="8971367290659962837" xfId="3" hidden="0"/>
+    <cellStyle name="-510541263188976588" xfId="1" hidden="0"/>
+    <cellStyle name="-933025415188404373" xfId="2" hidden="0"/>
+    <cellStyle name="1765305338777375516" xfId="3" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -481,7 +481,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:FA6"/>
+  <dimension ref="A1:FV7"/>
   <sheetViews>
     <sheetView rightToLeft="0" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,7 +489,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="19.5" customWidth="1" min="157" max="157"/>
+    <col width="19.5" customWidth="1" min="178" max="178"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -900,380 +900,485 @@
       </c>
       <c r="CD1" s="1" t="inlineStr">
         <is>
+          <t>dbmsDeployment.DBAAS.planetscaleInstance.region</t>
+        </is>
+      </c>
+      <c r="CE1" s="1" t="inlineStr">
+        <is>
+          <t>dbmsDeployment.DBAAS.planetscaleInstance.plan</t>
+        </is>
+      </c>
+      <c r="CF1" s="1" t="inlineStr">
+        <is>
+          <t>dbmsDeployment.DBAAS.planetscaleInstance.clusterSize</t>
+        </is>
+      </c>
+      <c r="CG1" s="1" t="inlineStr">
+        <is>
+          <t>benchmark.ycsb.workload.loadBatchSize</t>
+        </is>
+      </c>
+      <c r="CH1" s="1" t="inlineStr">
+        <is>
+          <t>benchmark.ycsb.workload.runBatchSize</t>
+        </is>
+      </c>
+      <c r="CI1" s="1" t="inlineStr">
+        <is>
           <t>actual_executions</t>
         </is>
       </c>
-      <c r="CE1" s="1" t="inlineStr">
+      <c r="CJ1" s="1" t="inlineStr">
         <is>
           <t>load_throughput_avg_std</t>
         </is>
       </c>
-      <c r="CF1" s="1" t="inlineStr">
+      <c r="CK1" s="1" t="inlineStr">
         <is>
           <t>run_throughput_avg_std</t>
         </is>
       </c>
-      <c r="CG1" s="1" t="inlineStr">
+      <c r="CL1" s="1" t="inlineStr">
+        <is>
+          <t>dbaas_deployment_time_std</t>
+        </is>
+      </c>
+      <c r="CM1" s="1" t="inlineStr">
         <is>
           <t>load_insert_avg_latency_avg_std</t>
         </is>
       </c>
-      <c r="CH1" s="1" t="inlineStr">
+      <c r="CN1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_90th_avg_std</t>
         </is>
       </c>
-      <c r="CI1" s="1" t="inlineStr">
+      <c r="CO1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_95th_avg_std</t>
         </is>
       </c>
-      <c r="CJ1" s="1" t="inlineStr">
+      <c r="CP1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_99th_avg_std</t>
         </is>
       </c>
-      <c r="CK1" s="1" t="inlineStr">
+      <c r="CQ1" s="1" t="inlineStr">
         <is>
           <t>run_insert_avg_latency_avg_std</t>
         </is>
       </c>
-      <c r="CL1" s="1" t="inlineStr">
+      <c r="CR1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_90th_avg_std</t>
         </is>
       </c>
-      <c r="CM1" s="1" t="inlineStr">
+      <c r="CS1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_95th_avg_std</t>
         </is>
       </c>
-      <c r="CN1" s="1" t="inlineStr">
+      <c r="CT1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_99th_avg_std</t>
         </is>
       </c>
-      <c r="CO1" s="1" t="inlineStr">
+      <c r="CU1" s="1" t="inlineStr">
         <is>
           <t>run_read_avg_latency_avg_std</t>
         </is>
       </c>
-      <c r="CP1" s="1" t="inlineStr">
+      <c r="CV1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_90th_avg_std</t>
         </is>
       </c>
-      <c r="CQ1" s="1" t="inlineStr">
+      <c r="CW1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_95th_avg_std</t>
         </is>
       </c>
-      <c r="CR1" s="1" t="inlineStr">
+      <c r="CX1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_99th_avg_std</t>
         </is>
       </c>
-      <c r="CS1" s="1" t="inlineStr">
+      <c r="CY1" s="1" t="inlineStr">
         <is>
           <t>run_update_avg_latency_avg_std</t>
         </is>
       </c>
-      <c r="CT1" s="1" t="inlineStr">
+      <c r="CZ1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_90th_avg_std</t>
         </is>
       </c>
-      <c r="CU1" s="1" t="inlineStr">
+      <c r="DA1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_95th_avg_std</t>
         </is>
       </c>
-      <c r="CV1" s="1" t="inlineStr">
+      <c r="DB1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_99th_avg_std</t>
         </is>
       </c>
-      <c r="CW1" s="1" t="inlineStr">
+      <c r="DC1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_avg_latency_avg_std</t>
+        </is>
+      </c>
+      <c r="DD1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_90th_avg_std</t>
+        </is>
+      </c>
+      <c r="DE1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_95th_avg_std</t>
+        </is>
+      </c>
+      <c r="DF1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_99th_avg_std</t>
+        </is>
+      </c>
+      <c r="DG1" s="1" t="inlineStr">
         <is>
           <t>run_delete_avg_latency_avg_std</t>
         </is>
       </c>
-      <c r="CX1" s="1" t="inlineStr">
+      <c r="DH1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_90th_avg_std</t>
         </is>
       </c>
-      <c r="CY1" s="1" t="inlineStr">
+      <c r="DI1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_95th_avg_std</t>
         </is>
       </c>
-      <c r="CZ1" s="1" t="inlineStr">
+      <c r="DJ1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_99th_avg_std</t>
         </is>
       </c>
-      <c r="DA1" s="1" t="inlineStr">
+      <c r="DK1" s="1" t="inlineStr">
         <is>
           <t>load_throughput_avg_mean</t>
         </is>
       </c>
-      <c r="DB1" s="1" t="inlineStr">
+      <c r="DL1" s="1" t="inlineStr">
         <is>
           <t>run_throughput_avg_mean</t>
         </is>
       </c>
-      <c r="DC1" s="1" t="inlineStr">
+      <c r="DM1" s="1" t="inlineStr">
+        <is>
+          <t>dbaas_deployment_time_mean</t>
+        </is>
+      </c>
+      <c r="DN1" s="1" t="inlineStr">
         <is>
           <t>load_insert_avg_latency_avg_mean</t>
         </is>
       </c>
-      <c r="DD1" s="1" t="inlineStr">
+      <c r="DO1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_90th_avg_mean</t>
         </is>
       </c>
-      <c r="DE1" s="1" t="inlineStr">
+      <c r="DP1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_95th_avg_mean</t>
         </is>
       </c>
-      <c r="DF1" s="1" t="inlineStr">
+      <c r="DQ1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_99th_avg_mean</t>
         </is>
       </c>
-      <c r="DG1" s="1" t="inlineStr">
+      <c r="DR1" s="1" t="inlineStr">
         <is>
           <t>run_insert_avg_latency_avg_mean</t>
         </is>
       </c>
-      <c r="DH1" s="1" t="inlineStr">
+      <c r="DS1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_90th_avg_mean</t>
         </is>
       </c>
-      <c r="DI1" s="1" t="inlineStr">
+      <c r="DT1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_95th_avg_mean</t>
         </is>
       </c>
-      <c r="DJ1" s="1" t="inlineStr">
+      <c r="DU1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_99th_avg_mean</t>
         </is>
       </c>
-      <c r="DK1" s="1" t="inlineStr">
+      <c r="DV1" s="1" t="inlineStr">
         <is>
           <t>run_read_avg_latency_avg_mean</t>
         </is>
       </c>
-      <c r="DL1" s="1" t="inlineStr">
+      <c r="DW1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_90th_avg_mean</t>
         </is>
       </c>
-      <c r="DM1" s="1" t="inlineStr">
+      <c r="DX1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_95th_avg_mean</t>
         </is>
       </c>
-      <c r="DN1" s="1" t="inlineStr">
+      <c r="DY1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_99th_avg_mean</t>
         </is>
       </c>
-      <c r="DO1" s="1" t="inlineStr">
+      <c r="DZ1" s="1" t="inlineStr">
         <is>
           <t>run_update_avg_latency_avg_mean</t>
         </is>
       </c>
-      <c r="DP1" s="1" t="inlineStr">
+      <c r="EA1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_90th_avg_mean</t>
         </is>
       </c>
-      <c r="DQ1" s="1" t="inlineStr">
+      <c r="EB1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_95th_avg_mean</t>
         </is>
       </c>
-      <c r="DR1" s="1" t="inlineStr">
+      <c r="EC1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_99th_avg_mean</t>
         </is>
       </c>
-      <c r="DS1" s="1" t="inlineStr">
+      <c r="ED1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_avg_latency_avg_mean</t>
+        </is>
+      </c>
+      <c r="EE1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_90th_avg_mean</t>
+        </is>
+      </c>
+      <c r="EF1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_95th_avg_mean</t>
+        </is>
+      </c>
+      <c r="EG1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_99th_avg_mean</t>
+        </is>
+      </c>
+      <c r="EH1" s="1" t="inlineStr">
         <is>
           <t>run_delete_avg_latency_avg_mean</t>
         </is>
       </c>
-      <c r="DT1" s="1" t="inlineStr">
+      <c r="EI1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_90th_avg_mean</t>
         </is>
       </c>
-      <c r="DU1" s="1" t="inlineStr">
+      <c r="EJ1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_95th_avg_mean</t>
         </is>
       </c>
-      <c r="DV1" s="1" t="inlineStr">
+      <c r="EK1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_99th_avg_mean</t>
         </is>
       </c>
-      <c r="DW1" s="1" t="inlineStr">
+      <c r="EL1" s="1" t="inlineStr">
         <is>
           <t>load_throughput_avg_cv</t>
         </is>
       </c>
-      <c r="DX1" s="1" t="inlineStr">
+      <c r="EM1" s="1" t="inlineStr">
         <is>
           <t>run_throughput_avg_cv</t>
         </is>
       </c>
-      <c r="DY1" s="1" t="inlineStr">
+      <c r="EN1" s="1" t="inlineStr">
+        <is>
+          <t>dbaas_deployment_time_cv</t>
+        </is>
+      </c>
+      <c r="EO1" s="1" t="inlineStr">
         <is>
           <t>load_insert_avg_latency_avg_cv</t>
         </is>
       </c>
-      <c r="DZ1" s="1" t="inlineStr">
+      <c r="EP1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_90th_avg_cv</t>
         </is>
       </c>
-      <c r="EA1" s="1" t="inlineStr">
+      <c r="EQ1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_95th_avg_cv</t>
         </is>
       </c>
-      <c r="EB1" s="1" t="inlineStr">
+      <c r="ER1" s="1" t="inlineStr">
         <is>
           <t>load_insert_latency_99th_avg_cv</t>
         </is>
       </c>
-      <c r="EC1" s="1" t="inlineStr">
+      <c r="ES1" s="1" t="inlineStr">
         <is>
           <t>run_insert_avg_latency_avg_cv</t>
         </is>
       </c>
-      <c r="ED1" s="1" t="inlineStr">
+      <c r="ET1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_90th_avg_cv</t>
         </is>
       </c>
-      <c r="EE1" s="1" t="inlineStr">
+      <c r="EU1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_95th_avg_cv</t>
         </is>
       </c>
-      <c r="EF1" s="1" t="inlineStr">
+      <c r="EV1" s="1" t="inlineStr">
         <is>
           <t>run_insert_latency_99th_avg_cv</t>
         </is>
       </c>
-      <c r="EG1" s="1" t="inlineStr">
+      <c r="EW1" s="1" t="inlineStr">
         <is>
           <t>run_read_avg_latency_avg_cv</t>
         </is>
       </c>
-      <c r="EH1" s="1" t="inlineStr">
+      <c r="EX1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_90th_avg_cv</t>
         </is>
       </c>
-      <c r="EI1" s="1" t="inlineStr">
+      <c r="EY1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_95th_avg_cv</t>
         </is>
       </c>
-      <c r="EJ1" s="1" t="inlineStr">
+      <c r="EZ1" s="1" t="inlineStr">
         <is>
           <t>run_read_latency_99th_avg_cv</t>
         </is>
       </c>
-      <c r="EK1" s="1" t="inlineStr">
+      <c r="FA1" s="1" t="inlineStr">
         <is>
           <t>run_update_avg_latency_avg_cv</t>
         </is>
       </c>
-      <c r="EL1" s="1" t="inlineStr">
+      <c r="FB1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_90th_avg_cv</t>
         </is>
       </c>
-      <c r="EM1" s="1" t="inlineStr">
+      <c r="FC1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_95th_avg_cv</t>
         </is>
       </c>
-      <c r="EN1" s="1" t="inlineStr">
+      <c r="FD1" s="1" t="inlineStr">
         <is>
           <t>run_update_latency_99th_avg_cv</t>
         </is>
       </c>
-      <c r="EO1" s="1" t="inlineStr">
+      <c r="FE1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_avg_latency_avg_cv</t>
+        </is>
+      </c>
+      <c r="FF1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_90th_avg_cv</t>
+        </is>
+      </c>
+      <c r="FG1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_95th_avg_cv</t>
+        </is>
+      </c>
+      <c r="FH1" s="1" t="inlineStr">
+        <is>
+          <t>run_scan_latency_99th_avg_cv</t>
+        </is>
+      </c>
+      <c r="FI1" s="1" t="inlineStr">
         <is>
           <t>run_delete_avg_latency_avg_cv</t>
         </is>
       </c>
-      <c r="EP1" s="1" t="inlineStr">
+      <c r="FJ1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_90th_avg_cv</t>
         </is>
       </c>
-      <c r="EQ1" s="1" t="inlineStr">
+      <c r="FK1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_95th_avg_cv</t>
         </is>
       </c>
-      <c r="ER1" s="1" t="inlineStr">
+      <c r="FL1" s="1" t="inlineStr">
         <is>
           <t>run_delete_latency_99th_avg_cv</t>
         </is>
       </c>
-      <c r="ES1" s="1" t="inlineStr">
+      <c r="FM1" s="1" t="inlineStr">
         <is>
           <t>source.directory</t>
         </is>
       </c>
-      <c r="ET1" s="1" t="inlineStr">
+      <c r="FN1" s="1" t="inlineStr">
         <is>
           <t>cloud.costs</t>
         </is>
       </c>
-      <c r="EU1" s="1" t="inlineStr">
+      <c r="FO1" s="1" t="inlineStr">
         <is>
           <t>throughput/euro</t>
         </is>
       </c>
-      <c r="EV1" s="1" t="inlineStr">
+      <c r="FP1" s="1" t="inlineStr">
         <is>
           <t>benchAnt_score_cloud_costs</t>
         </is>
       </c>
-      <c r="EW1" s="1" t="inlineStr">
+      <c r="FQ1" s="1" t="inlineStr">
         <is>
           <t>benchAnt_score_throughput</t>
         </is>
       </c>
-      <c r="EX1" s="1" t="inlineStr">
+      <c r="FR1" s="1" t="inlineStr">
         <is>
           <t>benchAnt_score_insert_latency_95</t>
         </is>
       </c>
-      <c r="EY1" s="1" t="inlineStr">
+      <c r="FS1" s="1" t="inlineStr">
         <is>
           <t>benchAnt_score_read_latency_95</t>
         </is>
       </c>
-      <c r="EZ1" s="1" t="inlineStr">
+      <c r="FT1" s="1" t="inlineStr">
         <is>
           <t>benchAnt_score_update_latency_95</t>
         </is>
       </c>
-      <c r="FA1" s="1" t="inlineStr">
+      <c r="FU1" s="1" t="inlineStr">
+        <is>
+          <t>benchAnt_score_scan_latency_95</t>
+        </is>
+      </c>
+      <c r="FV1" s="1" t="inlineStr">
         <is>
           <t>benchAnt_score_total</t>
         </is>
@@ -1531,187 +1636,216 @@
       <c r="CA2" s="2" t="inlineStr"/>
       <c r="CB2" s="2" t="inlineStr"/>
       <c r="CC2" s="2" t="inlineStr"/>
-      <c r="CD2" s="2" t="n">
+      <c r="CD2" s="2" t="inlineStr"/>
+      <c r="CE2" s="2" t="inlineStr"/>
+      <c r="CF2" s="2" t="inlineStr"/>
+      <c r="CG2" s="2" t="inlineStr"/>
+      <c r="CH2" s="2" t="inlineStr"/>
+      <c r="CI2" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="CE2" s="2" t="n">
+      <c r="CJ2" s="2" t="n">
         <v>300.7462571976534</v>
       </c>
-      <c r="CF2" s="2" t="n">
+      <c r="CK2" s="2" t="n">
         <v>241.7986960368624</v>
       </c>
-      <c r="CG2" s="2" t="n">
+      <c r="CL2" s="2" t="n">
+        <v>2.058191217400535</v>
+      </c>
+      <c r="CM2" s="2" t="n">
         <v>2.227352440591724</v>
       </c>
-      <c r="CH2" s="2" t="n">
+      <c r="CN2" s="2" t="n">
         <v>4.186583171294884e-05</v>
       </c>
-      <c r="CI2" s="2" t="n">
+      <c r="CO2" s="2" t="n">
         <v>0.0004714045207910315</v>
       </c>
-      <c r="CJ2" s="2" t="n">
+      <c r="CP2" s="2" t="n">
         <v>0.006480740698407861</v>
       </c>
-      <c r="CK2" s="2" t="n">
+      <c r="CQ2" s="2" t="n">
         <v>1.373061752532935</v>
       </c>
-      <c r="CL2" s="2" t="n">
+      <c r="CR2" s="2" t="n">
         <v>1.447091962271496</v>
       </c>
-      <c r="CM2" s="2" t="n">
+      <c r="CS2" s="2" t="n">
         <v>1.342814291785063</v>
       </c>
-      <c r="CN2" s="2" t="n">
+      <c r="CT2" s="2" t="n">
         <v>14.94207743997541</v>
       </c>
-      <c r="CO2" s="2" t="n">
+      <c r="CU2" s="2" t="n">
         <v>0.07137280100547136</v>
       </c>
-      <c r="CP2" s="2" t="n">
+      <c r="CV2" s="2" t="n">
         <v>0.08719934226010616</v>
       </c>
-      <c r="CQ2" s="2" t="n">
+      <c r="CW2" s="2" t="n">
         <v>0.1215711954187979</v>
       </c>
-      <c r="CR2" s="2" t="n">
+      <c r="CX2" s="2" t="n">
         <v>0.9373854893028564</v>
       </c>
-      <c r="CS2" s="2" t="inlineStr"/>
-      <c r="CT2" s="2" t="inlineStr"/>
-      <c r="CU2" s="2" t="inlineStr"/>
-      <c r="CV2" s="2" t="inlineStr"/>
-      <c r="CW2" s="2" t="inlineStr"/>
-      <c r="CX2" s="2" t="inlineStr"/>
       <c r="CY2" s="2" t="inlineStr"/>
       <c r="CZ2" s="2" t="inlineStr"/>
-      <c r="DA2" s="2" t="n">
+      <c r="DA2" s="2" t="inlineStr"/>
+      <c r="DB2" s="2" t="inlineStr"/>
+      <c r="DC2" s="2" t="inlineStr"/>
+      <c r="DD2" s="2" t="inlineStr"/>
+      <c r="DE2" s="2" t="inlineStr"/>
+      <c r="DF2" s="2" t="inlineStr"/>
+      <c r="DG2" s="2" t="inlineStr"/>
+      <c r="DH2" s="2" t="inlineStr"/>
+      <c r="DI2" s="2" t="inlineStr"/>
+      <c r="DJ2" s="2" t="inlineStr"/>
+      <c r="DK2" s="2" t="n">
         <v>3629.615143691823</v>
       </c>
-      <c r="DB2" s="2" t="n">
+      <c r="DL2" s="2" t="n">
         <v>5737.647446380336</v>
       </c>
-      <c r="DC2" s="2" t="n">
+      <c r="DM2" s="2" t="n">
+        <v>203.045717</v>
+      </c>
+      <c r="DN2" s="2" t="n">
         <v>27.30575755136667</v>
       </c>
-      <c r="DD2" s="2" t="n">
+      <c r="DO2" s="2" t="n">
         <v>0.009905088777802194</v>
       </c>
-      <c r="DE2" s="2" t="n">
+      <c r="DP2" s="2" t="n">
         <v>0.01166666666666667</v>
       </c>
-      <c r="DF2" s="2" t="n">
+      <c r="DQ2" s="2" t="n">
         <v>0.031</v>
       </c>
-      <c r="DG2" s="2" t="n">
+      <c r="DR2" s="2" t="n">
         <v>32.67779222750529</v>
       </c>
-      <c r="DH2" s="2" t="n">
+      <c r="DS2" s="2" t="n">
         <v>51.6885260115607</v>
       </c>
-      <c r="DI2" s="2" t="n">
+      <c r="DT2" s="2" t="n">
         <v>64.36166666666666</v>
       </c>
-      <c r="DJ2" s="2" t="n">
+      <c r="DU2" s="2" t="n">
         <v>138.8576666666667</v>
       </c>
-      <c r="DK2" s="2" t="n">
+      <c r="DV2" s="2" t="n">
         <v>1.769345806030046</v>
       </c>
-      <c r="DL2" s="2" t="n">
+      <c r="DW2" s="2" t="n">
         <v>2.561483622350675</v>
       </c>
-      <c r="DM2" s="2" t="n">
+      <c r="DX2" s="2" t="n">
         <v>3.340333333333334</v>
       </c>
-      <c r="DN2" s="2" t="n">
+      <c r="DY2" s="2" t="n">
         <v>10.38833333333333</v>
       </c>
-      <c r="DO2" s="2" t="inlineStr"/>
-      <c r="DP2" s="2" t="inlineStr"/>
-      <c r="DQ2" s="2" t="inlineStr"/>
-      <c r="DR2" s="2" t="inlineStr"/>
-      <c r="DS2" s="2" t="inlineStr"/>
-      <c r="DT2" s="2" t="inlineStr"/>
-      <c r="DU2" s="2" t="inlineStr"/>
-      <c r="DV2" s="2" t="inlineStr"/>
-      <c r="DW2" s="2" t="n">
+      <c r="DZ2" s="2" t="inlineStr"/>
+      <c r="EA2" s="2" t="inlineStr"/>
+      <c r="EB2" s="2" t="inlineStr"/>
+      <c r="EC2" s="2" t="inlineStr"/>
+      <c r="ED2" s="2" t="inlineStr"/>
+      <c r="EE2" s="2" t="inlineStr"/>
+      <c r="EF2" s="2" t="inlineStr"/>
+      <c r="EG2" s="2" t="inlineStr"/>
+      <c r="EH2" s="2" t="inlineStr"/>
+      <c r="EI2" s="2" t="inlineStr"/>
+      <c r="EJ2" s="2" t="inlineStr"/>
+      <c r="EK2" s="2" t="inlineStr"/>
+      <c r="EL2" s="2" t="n">
         <v>0.08285899338951754</v>
       </c>
-      <c r="DX2" s="2" t="n">
+      <c r="EM2" s="2" t="n">
         <v>0.04214248057178975</v>
       </c>
-      <c r="DY2" s="2" t="n">
+      <c r="EN2" s="2" t="n">
+        <v>0.01013659016210884</v>
+      </c>
+      <c r="EO2" s="2" t="n">
         <v>8.157079826119837e-05</v>
       </c>
-      <c r="DZ2" s="2" t="n">
+      <c r="EP2" s="2" t="n">
         <v>4.226699290850608e-06</v>
       </c>
-      <c r="EA2" s="2" t="n">
+      <c r="EQ2" s="2" t="n">
         <v>4.040610178208841e-05</v>
       </c>
-      <c r="EB2" s="2" t="n">
+      <c r="ER2" s="2" t="n">
         <v>0.0002090561515615439</v>
       </c>
-      <c r="EC2" s="2" t="n">
+      <c r="ES2" s="2" t="n">
         <v>4.201819214020255e-05</v>
       </c>
-      <c r="ED2" s="2" t="n">
+      <c r="ET2" s="2" t="n">
         <v>2.79963867019121e-05</v>
       </c>
-      <c r="EE2" s="2" t="n">
+      <c r="EU2" s="2" t="n">
         <v>2.086357239223755e-05</v>
       </c>
-      <c r="EF2" s="2" t="n">
+      <c r="EV2" s="2" t="n">
         <v>0.0001076071476546157</v>
       </c>
-      <c r="EG2" s="2" t="n">
+      <c r="EW2" s="2" t="n">
         <v>4.033852555121118e-05</v>
       </c>
-      <c r="EH2" s="2" t="n">
+      <c r="EX2" s="2" t="n">
         <v>3.404251407240437e-05</v>
       </c>
-      <c r="EI2" s="2" t="n">
+      <c r="EY2" s="2" t="n">
         <v>3.639492927416364e-05</v>
       </c>
-      <c r="EJ2" s="2" t="n">
+      <c r="EZ2" s="2" t="n">
         <v>9.023444466255637e-05</v>
       </c>
-      <c r="EK2" s="2" t="inlineStr"/>
-      <c r="EL2" s="2" t="inlineStr"/>
-      <c r="EM2" s="2" t="inlineStr"/>
-      <c r="EN2" s="2" t="inlineStr"/>
-      <c r="EO2" s="2" t="inlineStr"/>
-      <c r="EP2" s="2" t="inlineStr"/>
-      <c r="EQ2" s="2" t="inlineStr"/>
-      <c r="ER2" s="2" t="inlineStr"/>
-      <c r="ES2" s="2" t="inlineStr">
+      <c r="FA2" s="2" t="inlineStr"/>
+      <c r="FB2" s="2" t="inlineStr"/>
+      <c r="FC2" s="2" t="inlineStr"/>
+      <c r="FD2" s="2" t="inlineStr"/>
+      <c r="FE2" s="2" t="inlineStr"/>
+      <c r="FF2" s="2" t="inlineStr"/>
+      <c r="FG2" s="2" t="inlineStr"/>
+      <c r="FH2" s="2" t="inlineStr"/>
+      <c r="FI2" s="2" t="inlineStr"/>
+      <c r="FJ2" s="2" t="inlineStr"/>
+      <c r="FK2" s="2" t="inlineStr"/>
+      <c r="FL2" s="2" t="inlineStr"/>
+      <c r="FM2" s="2" t="inlineStr">
         <is>
           <t>['dbaas-navigator_ycsb_mariadb-azure_0_89i6Iw3A', 'dbaas-navigator_ycsb_mariadb-azure_0_eNzOvb0P', 'dbaas-navigator_ycsb_mariadb-azure_1_NHhQzp6b']</t>
         </is>
       </c>
-      <c r="ET2" s="2" t="n">
+      <c r="FN2" s="2" t="n">
         <v>997.01</v>
       </c>
-      <c r="EU2" s="2" t="n">
+      <c r="FO2" s="2" t="n">
         <v>5.754854461219382</v>
       </c>
-      <c r="EV2" s="2" t="n">
+      <c r="FP2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EW2" s="2" t="n">
+      <c r="FQ2" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="EX2" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="EY2" s="2" t="n">
+      <c r="FR2" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="FS2" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EZ2" s="2" t="n">
+      <c r="FT2" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="FA2" s="3" t="n">
-        <v>16</v>
+      <c r="FU2" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FV2" s="3" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -1972,186 +2106,215 @@
       <c r="CA3" s="2" t="inlineStr"/>
       <c r="CB3" s="2" t="inlineStr"/>
       <c r="CC3" s="2" t="inlineStr"/>
-      <c r="CD3" s="2" t="n">
+      <c r="CD3" s="2" t="inlineStr"/>
+      <c r="CE3" s="2" t="inlineStr"/>
+      <c r="CF3" s="2" t="inlineStr"/>
+      <c r="CG3" s="2" t="inlineStr"/>
+      <c r="CH3" s="2" t="inlineStr"/>
+      <c r="CI3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="CE3" s="2" t="n">
+      <c r="CJ3" s="2" t="n">
         <v>109.2676095492902</v>
       </c>
-      <c r="CF3" s="2" t="n">
+      <c r="CK3" s="2" t="n">
         <v>238.1498218528275</v>
       </c>
-      <c r="CG3" s="2" t="n">
+      <c r="CL3" s="2" t="n">
+        <v>28.15944127040375</v>
+      </c>
+      <c r="CM3" s="2" t="n">
         <v>0.06580735454412714</v>
       </c>
-      <c r="CH3" s="2" t="n">
+      <c r="CN3" s="2" t="n">
         <v>0.0006581185093855106</v>
       </c>
-      <c r="CI3" s="2" t="n">
+      <c r="CO3" s="2" t="n">
         <v>0.0008164965809277261</v>
       </c>
-      <c r="CJ3" s="2" t="n">
+      <c r="CP3" s="2" t="n">
         <v>0.0004714045207910321</v>
       </c>
-      <c r="CK3" s="2" t="n">
+      <c r="CQ3" s="2" t="n">
         <v>0.5141190702875607</v>
       </c>
-      <c r="CL3" s="2" t="n">
+      <c r="CR3" s="2" t="n">
         <v>6.293446641684089</v>
       </c>
-      <c r="CM3" s="2" t="n">
+      <c r="CS3" s="2" t="n">
         <v>0.4676332846247028</v>
       </c>
-      <c r="CN3" s="2" t="n">
+      <c r="CT3" s="2" t="n">
         <v>4.489361647272361</v>
       </c>
-      <c r="CO3" s="2" t="n">
+      <c r="CU3" s="2" t="n">
         <v>0.2674150621061222</v>
       </c>
-      <c r="CP3" s="2" t="n">
+      <c r="CV3" s="2" t="n">
         <v>0.1570832322149721</v>
       </c>
-      <c r="CQ3" s="2" t="n">
+      <c r="CW3" s="2" t="n">
         <v>0.1188724806953513</v>
       </c>
-      <c r="CR3" s="2" t="n">
+      <c r="CX3" s="2" t="n">
         <v>0.4204167244796789</v>
       </c>
-      <c r="CS3" s="2" t="inlineStr"/>
-      <c r="CT3" s="2" t="inlineStr"/>
-      <c r="CU3" s="2" t="inlineStr"/>
-      <c r="CV3" s="2" t="inlineStr"/>
-      <c r="CW3" s="2" t="inlineStr"/>
-      <c r="CX3" s="2" t="inlineStr"/>
       <c r="CY3" s="2" t="inlineStr"/>
       <c r="CZ3" s="2" t="inlineStr"/>
-      <c r="DA3" s="2" t="n">
+      <c r="DA3" s="2" t="inlineStr"/>
+      <c r="DB3" s="2" t="inlineStr"/>
+      <c r="DC3" s="2" t="inlineStr"/>
+      <c r="DD3" s="2" t="inlineStr"/>
+      <c r="DE3" s="2" t="inlineStr"/>
+      <c r="DF3" s="2" t="inlineStr"/>
+      <c r="DG3" s="2" t="inlineStr"/>
+      <c r="DH3" s="2" t="inlineStr"/>
+      <c r="DI3" s="2" t="inlineStr"/>
+      <c r="DJ3" s="2" t="inlineStr"/>
+      <c r="DK3" s="2" t="n">
         <v>12308.30575698829</v>
       </c>
-      <c r="DB3" s="2" t="n">
+      <c r="DL3" s="2" t="n">
         <v>8863.13330367148</v>
       </c>
-      <c r="DC3" s="2" t="n">
+      <c r="DM3" s="2" t="n">
+        <v>967.2113006666667</v>
+      </c>
+      <c r="DN3" s="2" t="n">
         <v>8.024581246199999</v>
       </c>
-      <c r="DD3" s="2" t="n">
+      <c r="DO3" s="2" t="n">
         <v>0.01360380658436214</v>
       </c>
-      <c r="DE3" s="2" t="n">
+      <c r="DP3" s="2" t="n">
         <v>0.019</v>
       </c>
-      <c r="DF3" s="2" t="n">
+      <c r="DQ3" s="2" t="n">
         <v>0.02966666666666667</v>
       </c>
-      <c r="DG3" s="2" t="n">
+      <c r="DR3" s="2" t="n">
         <v>20.77666001524911</v>
       </c>
-      <c r="DH3" s="2" t="n">
+      <c r="DS3" s="2" t="n">
         <v>35.75246435452794</v>
       </c>
-      <c r="DI3" s="2" t="n">
+      <c r="DT3" s="2" t="n">
         <v>35.09233333333334</v>
       </c>
-      <c r="DJ3" s="2" t="n">
+      <c r="DU3" s="2" t="n">
         <v>63.775</v>
       </c>
-      <c r="DK3" s="2" t="n">
+      <c r="DV3" s="2" t="n">
         <v>1.483850886534895</v>
       </c>
-      <c r="DL3" s="2" t="n">
+      <c r="DW3" s="2" t="n">
         <v>2.574755298651252</v>
       </c>
-      <c r="DM3" s="2" t="n">
+      <c r="DX3" s="2" t="n">
         <v>3.565</v>
       </c>
-      <c r="DN3" s="2" t="n">
+      <c r="DY3" s="2" t="n">
         <v>7.625666666666667</v>
       </c>
-      <c r="DO3" s="2" t="inlineStr"/>
-      <c r="DP3" s="2" t="inlineStr"/>
-      <c r="DQ3" s="2" t="inlineStr"/>
-      <c r="DR3" s="2" t="inlineStr"/>
-      <c r="DS3" s="2" t="inlineStr"/>
-      <c r="DT3" s="2" t="inlineStr"/>
-      <c r="DU3" s="2" t="inlineStr"/>
-      <c r="DV3" s="2" t="inlineStr"/>
-      <c r="DW3" s="2" t="n">
+      <c r="DZ3" s="2" t="inlineStr"/>
+      <c r="EA3" s="2" t="inlineStr"/>
+      <c r="EB3" s="2" t="inlineStr"/>
+      <c r="EC3" s="2" t="inlineStr"/>
+      <c r="ED3" s="2" t="inlineStr"/>
+      <c r="EE3" s="2" t="inlineStr"/>
+      <c r="EF3" s="2" t="inlineStr"/>
+      <c r="EG3" s="2" t="inlineStr"/>
+      <c r="EH3" s="2" t="inlineStr"/>
+      <c r="EI3" s="2" t="inlineStr"/>
+      <c r="EJ3" s="2" t="inlineStr"/>
+      <c r="EK3" s="2" t="inlineStr"/>
+      <c r="EL3" s="2" t="n">
         <v>0.008877550794287935</v>
       </c>
-      <c r="DX3" s="2" t="n">
+      <c r="EM3" s="2" t="n">
         <v>0.02686971003292661</v>
       </c>
-      <c r="DY3" s="2" t="n">
+      <c r="EN3" s="2" t="n">
+        <v>0.02911405320739572</v>
+      </c>
+      <c r="EO3" s="2" t="n">
         <v>8.200721324279681e-06</v>
       </c>
-      <c r="DZ3" s="2" t="n">
+      <c r="EP3" s="2" t="n">
         <v>4.837752619491309e-05</v>
       </c>
-      <c r="EA3" s="2" t="n">
+      <c r="EQ3" s="2" t="n">
         <v>4.2973504259354e-05</v>
       </c>
-      <c r="EB3" s="2" t="n">
+      <c r="ER3" s="2" t="n">
         <v>1.5890040026664e-05</v>
       </c>
-      <c r="EC3" s="2" t="n">
+      <c r="ES3" s="2" t="n">
         <v>2.474502975503382e-05</v>
       </c>
-      <c r="ED3" s="2" t="n">
+      <c r="ET3" s="2" t="n">
         <v>0.0001760283313417819</v>
       </c>
-      <c r="EE3" s="2" t="n">
+      <c r="EU3" s="2" t="n">
         <v>1.332579626959458e-05</v>
       </c>
-      <c r="EF3" s="2" t="n">
+      <c r="EV3" s="2" t="n">
         <v>7.039375377926085e-05</v>
       </c>
-      <c r="EG3" s="2" t="n">
+      <c r="EW3" s="2" t="n">
         <v>0.0001802169372493976</v>
       </c>
-      <c r="EH3" s="2" t="n">
+      <c r="EX3" s="2" t="n">
         <v>6.100899464009564e-05</v>
       </c>
-      <c r="EI3" s="2" t="n">
+      <c r="EY3" s="2" t="n">
         <v>3.334431436054735e-05</v>
       </c>
-      <c r="EJ3" s="2" t="n">
+      <c r="EZ3" s="2" t="n">
         <v>5.513179933728359e-05</v>
       </c>
-      <c r="EK3" s="2" t="inlineStr"/>
-      <c r="EL3" s="2" t="inlineStr"/>
-      <c r="EM3" s="2" t="inlineStr"/>
-      <c r="EN3" s="2" t="inlineStr"/>
-      <c r="EO3" s="2" t="inlineStr"/>
-      <c r="EP3" s="2" t="inlineStr"/>
-      <c r="EQ3" s="2" t="inlineStr"/>
-      <c r="ER3" s="2" t="inlineStr"/>
-      <c r="ES3" s="2" t="inlineStr">
+      <c r="FA3" s="2" t="inlineStr"/>
+      <c r="FB3" s="2" t="inlineStr"/>
+      <c r="FC3" s="2" t="inlineStr"/>
+      <c r="FD3" s="2" t="inlineStr"/>
+      <c r="FE3" s="2" t="inlineStr"/>
+      <c r="FF3" s="2" t="inlineStr"/>
+      <c r="FG3" s="2" t="inlineStr"/>
+      <c r="FH3" s="2" t="inlineStr"/>
+      <c r="FI3" s="2" t="inlineStr"/>
+      <c r="FJ3" s="2" t="inlineStr"/>
+      <c r="FK3" s="2" t="inlineStr"/>
+      <c r="FL3" s="2" t="inlineStr"/>
+      <c r="FM3" s="2" t="inlineStr">
         <is>
           <t>['dbaas-navigator_ycsb_mariadb-rds-aws_0_TPtU1cum', 'dbaas-navigator_ycsb_mariadb-rds-aws_0_vTmFg6xd', 'dbaas-navigator_ycsb_mariadb-rds-aws_1_YOUUiDuH']</t>
         </is>
       </c>
-      <c r="ET3" s="2" t="n">
+      <c r="FN3" s="2" t="n">
         <v>2013.69</v>
       </c>
-      <c r="EU3" s="2" t="n">
+      <c r="FO3" s="2" t="n">
         <v>4.401438803227647</v>
       </c>
-      <c r="EV3" s="2" t="n">
+      <c r="FP3" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="EW3" s="2" t="n">
+      <c r="FQ3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EX3" s="2" t="n">
+      <c r="FR3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EY3" s="2" t="n">
+      <c r="FS3" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EZ3" s="2" t="n">
+      <c r="FT3" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="FA3" s="3" t="n">
+      <c r="FU3" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FV3" s="3" t="n">
         <v>18</v>
       </c>
     </row>
@@ -2415,186 +2578,215 @@
       <c r="CA4" s="2" t="inlineStr"/>
       <c r="CB4" s="2" t="inlineStr"/>
       <c r="CC4" s="2" t="inlineStr"/>
-      <c r="CD4" s="2" t="n">
+      <c r="CD4" s="2" t="inlineStr"/>
+      <c r="CE4" s="2" t="inlineStr"/>
+      <c r="CF4" s="2" t="inlineStr"/>
+      <c r="CG4" s="2" t="inlineStr"/>
+      <c r="CH4" s="2" t="inlineStr"/>
+      <c r="CI4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="CE4" s="2" t="n">
+      <c r="CJ4" s="2" t="n">
         <v>28.73709853244613</v>
       </c>
-      <c r="CF4" s="2" t="n">
+      <c r="CK4" s="2" t="n">
         <v>67.04266345299273</v>
       </c>
-      <c r="CG4" s="2" t="n">
+      <c r="CL4" s="2" t="n">
+        <v>103.9740570090817</v>
+      </c>
+      <c r="CM4" s="2" t="n">
         <v>0.5720957033056157</v>
       </c>
-      <c r="CH4" s="2" t="n">
+      <c r="CN4" s="2" t="n">
         <v>39.25212076071488</v>
       </c>
-      <c r="CI4" s="2" t="n">
+      <c r="CO4" s="2" t="n">
         <v>0.001632993161855452</v>
       </c>
-      <c r="CJ4" s="2" t="n">
+      <c r="CP4" s="2" t="n">
         <v>0.003091206165165236</v>
       </c>
-      <c r="CK4" s="2" t="n">
+      <c r="CQ4" s="2" t="n">
         <v>0.960939628591457</v>
       </c>
-      <c r="CL4" s="2" t="n">
+      <c r="CR4" s="2" t="n">
         <v>2.163777123058335</v>
       </c>
-      <c r="CM4" s="2" t="n">
+      <c r="CS4" s="2" t="n">
         <v>1.914540385807749</v>
       </c>
-      <c r="CN4" s="2" t="n">
+      <c r="CT4" s="2" t="n">
         <v>8.342833624667872</v>
       </c>
-      <c r="CO4" s="2" t="n">
+      <c r="CU4" s="2" t="n">
         <v>0.383538681524916</v>
       </c>
-      <c r="CP4" s="2" t="n">
+      <c r="CV4" s="2" t="n">
         <v>0.3323490658546632</v>
       </c>
-      <c r="CQ4" s="2" t="n">
+      <c r="CW4" s="2" t="n">
         <v>0.06402777175222928</v>
       </c>
-      <c r="CR4" s="2" t="n">
+      <c r="CX4" s="2" t="n">
         <v>0.7298292037639126</v>
       </c>
-      <c r="CS4" s="2" t="inlineStr"/>
-      <c r="CT4" s="2" t="inlineStr"/>
-      <c r="CU4" s="2" t="inlineStr"/>
-      <c r="CV4" s="2" t="inlineStr"/>
-      <c r="CW4" s="2" t="inlineStr"/>
-      <c r="CX4" s="2" t="inlineStr"/>
       <c r="CY4" s="2" t="inlineStr"/>
       <c r="CZ4" s="2" t="inlineStr"/>
-      <c r="DA4" s="2" t="n">
+      <c r="DA4" s="2" t="inlineStr"/>
+      <c r="DB4" s="2" t="inlineStr"/>
+      <c r="DC4" s="2" t="inlineStr"/>
+      <c r="DD4" s="2" t="inlineStr"/>
+      <c r="DE4" s="2" t="inlineStr"/>
+      <c r="DF4" s="2" t="inlineStr"/>
+      <c r="DG4" s="2" t="inlineStr"/>
+      <c r="DH4" s="2" t="inlineStr"/>
+      <c r="DI4" s="2" t="inlineStr"/>
+      <c r="DJ4" s="2" t="inlineStr"/>
+      <c r="DK4" s="2" t="n">
         <v>2301.67248390509</v>
       </c>
-      <c r="DB4" s="2" t="n">
+      <c r="DL4" s="2" t="n">
         <v>3869.735993529562</v>
       </c>
-      <c r="DC4" s="2" t="n">
+      <c r="DM4" s="2" t="n">
+        <v>1236.05332</v>
+      </c>
+      <c r="DN4" s="2" t="n">
         <v>43.24105787713333</v>
       </c>
-      <c r="DD4" s="2" t="n">
+      <c r="DO4" s="2" t="n">
         <v>55.16346773225559</v>
       </c>
-      <c r="DE4" s="2" t="n">
+      <c r="DP4" s="2" t="n">
         <v>0.06900000000000001</v>
       </c>
-      <c r="DF4" s="2" t="n">
+      <c r="DQ4" s="2" t="n">
         <v>0.08466666666666667</v>
       </c>
-      <c r="DG4" s="2" t="n">
+      <c r="DR4" s="2" t="n">
         <v>48.44677866680737</v>
       </c>
-      <c r="DH4" s="2" t="n">
+      <c r="DS4" s="2" t="n">
         <v>78.93800578034683</v>
       </c>
-      <c r="DI4" s="2" t="n">
+      <c r="DT4" s="2" t="n">
         <v>96.27633333333333</v>
       </c>
-      <c r="DJ4" s="2" t="n">
+      <c r="DU4" s="2" t="n">
         <v>197.9723333333334</v>
       </c>
-      <c r="DK4" s="2" t="n">
+      <c r="DV4" s="2" t="n">
         <v>2.542853316597432</v>
       </c>
-      <c r="DL4" s="2" t="n">
+      <c r="DW4" s="2" t="n">
         <v>4.351674373795761</v>
       </c>
-      <c r="DM4" s="2" t="n">
+      <c r="DX4" s="2" t="n">
         <v>7.293666666666667</v>
       </c>
-      <c r="DN4" s="2" t="n">
+      <c r="DY4" s="2" t="n">
         <v>28.351</v>
       </c>
-      <c r="DO4" s="2" t="inlineStr"/>
-      <c r="DP4" s="2" t="inlineStr"/>
-      <c r="DQ4" s="2" t="inlineStr"/>
-      <c r="DR4" s="2" t="inlineStr"/>
-      <c r="DS4" s="2" t="inlineStr"/>
-      <c r="DT4" s="2" t="inlineStr"/>
-      <c r="DU4" s="2" t="inlineStr"/>
-      <c r="DV4" s="2" t="inlineStr"/>
-      <c r="DW4" s="2" t="n">
+      <c r="DZ4" s="2" t="inlineStr"/>
+      <c r="EA4" s="2" t="inlineStr"/>
+      <c r="EB4" s="2" t="inlineStr"/>
+      <c r="EC4" s="2" t="inlineStr"/>
+      <c r="ED4" s="2" t="inlineStr"/>
+      <c r="EE4" s="2" t="inlineStr"/>
+      <c r="EF4" s="2" t="inlineStr"/>
+      <c r="EG4" s="2" t="inlineStr"/>
+      <c r="EH4" s="2" t="inlineStr"/>
+      <c r="EI4" s="2" t="inlineStr"/>
+      <c r="EJ4" s="2" t="inlineStr"/>
+      <c r="EK4" s="2" t="inlineStr"/>
+      <c r="EL4" s="2" t="n">
         <v>0.01248531176064193</v>
       </c>
-      <c r="DX4" s="2" t="n">
+      <c r="EM4" s="2" t="n">
         <v>0.01732486752716263</v>
       </c>
-      <c r="DY4" s="2" t="n">
+      <c r="EN4" s="2" t="n">
+        <v>0.08411777657705069</v>
+      </c>
+      <c r="EO4" s="2" t="n">
         <v>1.323038175733786e-05</v>
       </c>
-      <c r="DZ4" s="2" t="n">
+      <c r="EP4" s="2" t="n">
         <v>0.0007115600663691251</v>
       </c>
-      <c r="EA4" s="2" t="n">
+      <c r="EQ4" s="2" t="n">
         <v>2.366656756312249e-05</v>
       </c>
-      <c r="EB4" s="2" t="n">
+      <c r="ER4" s="2" t="n">
         <v>3.651030903738468e-05</v>
       </c>
-      <c r="EC4" s="2" t="n">
+      <c r="ES4" s="2" t="n">
         <v>1.983495404720957e-05</v>
       </c>
-      <c r="ED4" s="2" t="n">
+      <c r="ET4" s="2" t="n">
         <v>2.741109433495532e-05</v>
       </c>
-      <c r="EE4" s="2" t="n">
+      <c r="EU4" s="2" t="n">
         <v>1.98858880424862e-05</v>
       </c>
-      <c r="EF4" s="2" t="n">
+      <c r="EV4" s="2" t="n">
         <v>4.214141180333887e-05</v>
       </c>
-      <c r="EG4" s="2" t="n">
+      <c r="EW4" s="2" t="n">
         <v>0.0001508300455325223</v>
       </c>
-      <c r="EH4" s="2" t="n">
+      <c r="EX4" s="2" t="n">
         <v>7.637268722493377e-05</v>
       </c>
-      <c r="EI4" s="2" t="n">
+      <c r="EY4" s="2" t="n">
         <v>8.778543725455317e-06</v>
       </c>
-      <c r="EJ4" s="2" t="n">
+      <c r="EZ4" s="2" t="n">
         <v>2.5742626495147e-05</v>
       </c>
-      <c r="EK4" s="2" t="inlineStr"/>
-      <c r="EL4" s="2" t="inlineStr"/>
-      <c r="EM4" s="2" t="inlineStr"/>
-      <c r="EN4" s="2" t="inlineStr"/>
-      <c r="EO4" s="2" t="inlineStr"/>
-      <c r="EP4" s="2" t="inlineStr"/>
-      <c r="EQ4" s="2" t="inlineStr"/>
-      <c r="ER4" s="2" t="inlineStr"/>
-      <c r="ES4" s="2" t="inlineStr">
+      <c r="FA4" s="2" t="inlineStr"/>
+      <c r="FB4" s="2" t="inlineStr"/>
+      <c r="FC4" s="2" t="inlineStr"/>
+      <c r="FD4" s="2" t="inlineStr"/>
+      <c r="FE4" s="2" t="inlineStr"/>
+      <c r="FF4" s="2" t="inlineStr"/>
+      <c r="FG4" s="2" t="inlineStr"/>
+      <c r="FH4" s="2" t="inlineStr"/>
+      <c r="FI4" s="2" t="inlineStr"/>
+      <c r="FJ4" s="2" t="inlineStr"/>
+      <c r="FK4" s="2" t="inlineStr"/>
+      <c r="FL4" s="2" t="inlineStr"/>
+      <c r="FM4" s="2" t="inlineStr">
         <is>
           <t>['dbaas-navigator_ycsb_mysql-flexible-server-azure_0_sackyTNt', 'dbaas-navigator_ycsb_mysql-flexible-server-azure_0_YMOSyEHB', 'dbaas-navigator_ycsb_mysql-flexible-server-azure_1_Xti0Cm7e']</t>
         </is>
       </c>
-      <c r="ET4" s="2" t="n">
+      <c r="FN4" s="2" t="n">
         <v>1978.83</v>
       </c>
-      <c r="EU4" s="2" t="n">
+      <c r="FO4" s="2" t="n">
         <v>1.955567680664616</v>
       </c>
-      <c r="EV4" s="2" t="n">
+      <c r="FP4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="EW4" s="2" t="n">
+      <c r="FQ4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="EX4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="EY4" s="2" t="n">
+      <c r="FR4" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FS4" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="EZ4" s="2" t="n">
+      <c r="FT4" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="FA4" s="3" t="n">
+      <c r="FU4" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FV4" s="3" t="n">
         <v>5</v>
       </c>
     </row>
@@ -2856,187 +3048,216 @@
       <c r="CA5" s="2" t="inlineStr"/>
       <c r="CB5" s="2" t="inlineStr"/>
       <c r="CC5" s="2" t="inlineStr"/>
-      <c r="CD5" s="2" t="n">
+      <c r="CD5" s="2" t="inlineStr"/>
+      <c r="CE5" s="2" t="inlineStr"/>
+      <c r="CF5" s="2" t="inlineStr"/>
+      <c r="CG5" s="2" t="inlineStr"/>
+      <c r="CH5" s="2" t="inlineStr"/>
+      <c r="CI5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="CE5" s="2" t="n">
+      <c r="CJ5" s="2" t="n">
         <v>84.69455310752909</v>
       </c>
-      <c r="CF5" s="2" t="n">
+      <c r="CK5" s="2" t="n">
         <v>176.6392413428097</v>
       </c>
-      <c r="CG5" s="2" t="n">
+      <c r="CL5" s="2" t="n">
+        <v>28.45155130306304</v>
+      </c>
+      <c r="CM5" s="2" t="n">
         <v>0.9644165820033963</v>
       </c>
-      <c r="CH5" s="2" t="n">
+      <c r="CN5" s="2" t="n">
         <v>42.56413178781133</v>
       </c>
-      <c r="CI5" s="2" t="n">
+      <c r="CO5" s="2" t="n">
         <v>0.002494438257849293</v>
       </c>
-      <c r="CJ5" s="2" t="n">
+      <c r="CP5" s="2" t="n">
         <v>0.002054804667656327</v>
       </c>
-      <c r="CK5" s="2" t="n">
+      <c r="CQ5" s="2" t="n">
         <v>1.003783210274046</v>
       </c>
-      <c r="CL5" s="2" t="n">
+      <c r="CR5" s="2" t="n">
         <v>2.507423071669662</v>
       </c>
-      <c r="CM5" s="2" t="n">
+      <c r="CS5" s="2" t="n">
         <v>2.751048931266441</v>
       </c>
-      <c r="CN5" s="2" t="n">
+      <c r="CT5" s="2" t="n">
         <v>3.215747917151881</v>
       </c>
-      <c r="CO5" s="2" t="n">
+      <c r="CU5" s="2" t="n">
         <v>0.2203736743111106</v>
       </c>
-      <c r="CP5" s="2" t="n">
+      <c r="CV5" s="2" t="n">
         <v>0.5931816819569048</v>
       </c>
-      <c r="CQ5" s="2" t="n">
+      <c r="CW5" s="2" t="n">
         <v>1.154113801436699</v>
       </c>
-      <c r="CR5" s="2" t="n">
+      <c r="CX5" s="2" t="n">
         <v>2.513001923331271</v>
       </c>
-      <c r="CS5" s="2" t="inlineStr"/>
-      <c r="CT5" s="2" t="inlineStr"/>
-      <c r="CU5" s="2" t="inlineStr"/>
-      <c r="CV5" s="2" t="inlineStr"/>
-      <c r="CW5" s="2" t="inlineStr"/>
-      <c r="CX5" s="2" t="inlineStr"/>
       <c r="CY5" s="2" t="inlineStr"/>
       <c r="CZ5" s="2" t="inlineStr"/>
-      <c r="DA5" s="2" t="n">
+      <c r="DA5" s="2" t="inlineStr"/>
+      <c r="DB5" s="2" t="inlineStr"/>
+      <c r="DC5" s="2" t="inlineStr"/>
+      <c r="DD5" s="2" t="inlineStr"/>
+      <c r="DE5" s="2" t="inlineStr"/>
+      <c r="DF5" s="2" t="inlineStr"/>
+      <c r="DG5" s="2" t="inlineStr"/>
+      <c r="DH5" s="2" t="inlineStr"/>
+      <c r="DI5" s="2" t="inlineStr"/>
+      <c r="DJ5" s="2" t="inlineStr"/>
+      <c r="DK5" s="2" t="n">
         <v>2989.287711740119</v>
       </c>
-      <c r="DB5" s="2" t="n">
+      <c r="DL5" s="2" t="n">
         <v>5408.758231698112</v>
       </c>
-      <c r="DC5" s="2" t="n">
+      <c r="DM5" s="2" t="n">
+        <v>946.6241033333334</v>
+      </c>
+      <c r="DN5" s="2" t="n">
         <v>33.3250385282</v>
       </c>
-      <c r="DD5" s="2" t="n">
+      <c r="DO5" s="2" t="n">
         <v>154.8501483593677</v>
       </c>
-      <c r="DE5" s="2" t="n">
+      <c r="DP5" s="2" t="n">
         <v>0.09033333333333333</v>
       </c>
-      <c r="DF5" s="2" t="n">
+      <c r="DQ5" s="2" t="n">
         <v>0.1036666666666667</v>
       </c>
-      <c r="DG5" s="2" t="n">
+      <c r="DR5" s="2" t="n">
         <v>34.36721278599976</v>
       </c>
-      <c r="DH5" s="2" t="n">
+      <c r="DS5" s="2" t="n">
         <v>52.5074238921002</v>
       </c>
-      <c r="DI5" s="2" t="n">
+      <c r="DT5" s="2" t="n">
         <v>63.01766666666666</v>
       </c>
-      <c r="DJ5" s="2" t="n">
+      <c r="DU5" s="2" t="n">
         <v>91.711</v>
       </c>
-      <c r="DK5" s="2" t="n">
+      <c r="DV5" s="2" t="n">
         <v>2.176265449273559</v>
       </c>
-      <c r="DL5" s="2" t="n">
+      <c r="DW5" s="2" t="n">
         <v>4.243651252408478</v>
       </c>
-      <c r="DM5" s="2" t="n">
+      <c r="DX5" s="2" t="n">
         <v>6.151</v>
       </c>
-      <c r="DN5" s="2" t="n">
+      <c r="DY5" s="2" t="n">
         <v>19.455</v>
       </c>
-      <c r="DO5" s="2" t="inlineStr"/>
-      <c r="DP5" s="2" t="inlineStr"/>
-      <c r="DQ5" s="2" t="inlineStr"/>
-      <c r="DR5" s="2" t="inlineStr"/>
-      <c r="DS5" s="2" t="inlineStr"/>
-      <c r="DT5" s="2" t="inlineStr"/>
-      <c r="DU5" s="2" t="inlineStr"/>
-      <c r="DV5" s="2" t="inlineStr"/>
-      <c r="DW5" s="2" t="n">
+      <c r="DZ5" s="2" t="inlineStr"/>
+      <c r="EA5" s="2" t="inlineStr"/>
+      <c r="EB5" s="2" t="inlineStr"/>
+      <c r="EC5" s="2" t="inlineStr"/>
+      <c r="ED5" s="2" t="inlineStr"/>
+      <c r="EE5" s="2" t="inlineStr"/>
+      <c r="EF5" s="2" t="inlineStr"/>
+      <c r="EG5" s="2" t="inlineStr"/>
+      <c r="EH5" s="2" t="inlineStr"/>
+      <c r="EI5" s="2" t="inlineStr"/>
+      <c r="EJ5" s="2" t="inlineStr"/>
+      <c r="EK5" s="2" t="inlineStr"/>
+      <c r="EL5" s="2" t="n">
         <v>0.02833268700597135</v>
       </c>
-      <c r="DX5" s="2" t="n">
+      <c r="EM5" s="2" t="n">
         <v>0.03265800277550079</v>
       </c>
-      <c r="DY5" s="2" t="n">
+      <c r="EN5" s="2" t="n">
+        <v>0.03005580694900649</v>
+      </c>
+      <c r="EO5" s="2" t="n">
         <v>2.893969893500039e-05</v>
       </c>
-      <c r="DZ5" s="2" t="n">
+      <c r="EP5" s="2" t="n">
         <v>0.0002748730449326457</v>
       </c>
-      <c r="EA5" s="2" t="n">
+      <c r="EQ5" s="2" t="n">
         <v>2.761370765146819e-05</v>
       </c>
-      <c r="EB5" s="2" t="n">
+      <c r="ER5" s="2" t="n">
         <v>1.98212668905755e-05</v>
       </c>
-      <c r="EC5" s="2" t="n">
+      <c r="ES5" s="2" t="n">
         <v>2.920758271915957e-05</v>
       </c>
-      <c r="ED5" s="2" t="n">
+      <c r="ET5" s="2" t="n">
         <v>4.775368673241855e-05</v>
       </c>
-      <c r="EE5" s="2" t="n">
+      <c r="EU5" s="2" t="n">
         <v>4.365520141864621e-05</v>
       </c>
-      <c r="EF5" s="2" t="n">
+      <c r="EV5" s="2" t="n">
         <v>3.50639281782107e-05</v>
       </c>
-      <c r="EG5" s="2" t="n">
+      <c r="EW5" s="2" t="n">
         <v>0.000101262313558611</v>
       </c>
-      <c r="EH5" s="2" t="n">
+      <c r="EX5" s="2" t="n">
         <v>0.000139780968480915</v>
       </c>
-      <c r="EI5" s="2" t="n">
+      <c r="EY5" s="2" t="n">
         <v>0.0001876302717341406</v>
       </c>
-      <c r="EJ5" s="2" t="n">
+      <c r="EZ5" s="2" t="n">
         <v>0.0001291699780689422</v>
       </c>
-      <c r="EK5" s="2" t="inlineStr"/>
-      <c r="EL5" s="2" t="inlineStr"/>
-      <c r="EM5" s="2" t="inlineStr"/>
-      <c r="EN5" s="2" t="inlineStr"/>
-      <c r="EO5" s="2" t="inlineStr"/>
-      <c r="EP5" s="2" t="inlineStr"/>
-      <c r="EQ5" s="2" t="inlineStr"/>
-      <c r="ER5" s="2" t="inlineStr"/>
-      <c r="ES5" s="2" t="inlineStr">
+      <c r="FA5" s="2" t="inlineStr"/>
+      <c r="FB5" s="2" t="inlineStr"/>
+      <c r="FC5" s="2" t="inlineStr"/>
+      <c r="FD5" s="2" t="inlineStr"/>
+      <c r="FE5" s="2" t="inlineStr"/>
+      <c r="FF5" s="2" t="inlineStr"/>
+      <c r="FG5" s="2" t="inlineStr"/>
+      <c r="FH5" s="2" t="inlineStr"/>
+      <c r="FI5" s="2" t="inlineStr"/>
+      <c r="FJ5" s="2" t="inlineStr"/>
+      <c r="FK5" s="2" t="inlineStr"/>
+      <c r="FL5" s="2" t="inlineStr"/>
+      <c r="FM5" s="2" t="inlineStr">
         <is>
           <t>['dbaas-navigator_ycsb_mysql-rds-aws_0_H1TpCGQi', 'dbaas-navigator_ycsb_mysql-rds-aws_0_Pl0ZGbQq', 'dbaas-navigator_ycsb_mysql-rds-aws_1_dpN7i0aG']</t>
         </is>
       </c>
-      <c r="ET5" s="2" t="n">
+      <c r="FN5" s="2" t="n">
         <v>2013.69</v>
       </c>
-      <c r="EU5" s="2" t="n">
+      <c r="FO5" s="2" t="n">
         <v>2.685993490407219</v>
       </c>
-      <c r="EV5" s="2" t="n">
+      <c r="FP5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="EW5" s="2" t="n">
+      <c r="FQ5" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="EX5" s="2" t="n">
+      <c r="FR5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="FS5" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="EY5" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="EZ5" s="2" t="n">
+      <c r="FT5" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="FA5" s="3" t="n">
-        <v>11</v>
+      <c r="FU5" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FV5" s="3" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="6">
@@ -3299,187 +3520,682 @@
           <t>INNODB</t>
         </is>
       </c>
-      <c r="CD6" s="2" t="n">
+      <c r="CD6" s="2" t="inlineStr"/>
+      <c r="CE6" s="2" t="inlineStr"/>
+      <c r="CF6" s="2" t="inlineStr"/>
+      <c r="CG6" s="2" t="inlineStr"/>
+      <c r="CH6" s="2" t="inlineStr"/>
+      <c r="CI6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="CE6" s="2" t="n">
+      <c r="CJ6" s="2" t="n">
         <v>36.79548142547196</v>
       </c>
-      <c r="CF6" s="2" t="n">
+      <c r="CK6" s="2" t="n">
         <v>197.703267403576</v>
       </c>
-      <c r="CG6" s="2" t="n">
+      <c r="CL6" s="2" t="n">
+        <v>2.248221031919079</v>
+      </c>
+      <c r="CM6" s="2" t="n">
         <v>0.1623366559665249</v>
       </c>
-      <c r="CH6" s="2" t="n">
+      <c r="CN6" s="2" t="n">
         <v>0.003341539721682303</v>
       </c>
-      <c r="CI6" s="2" t="n">
+      <c r="CO6" s="2" t="n">
         <v>0.00524933858267454</v>
       </c>
-      <c r="CJ6" s="2" t="n">
+      <c r="CP6" s="2" t="n">
         <v>0.004642796092394705</v>
       </c>
-      <c r="CK6" s="2" t="n">
+      <c r="CQ6" s="2" t="n">
         <v>0.6679021431024005</v>
       </c>
-      <c r="CL6" s="2" t="n">
+      <c r="CR6" s="2" t="n">
         <v>1.924528883475515</v>
       </c>
-      <c r="CM6" s="2" t="n">
+      <c r="CS6" s="2" t="n">
         <v>2.221075615301939</v>
       </c>
-      <c r="CN6" s="2" t="n">
+      <c r="CT6" s="2" t="n">
         <v>2.391855811336089</v>
       </c>
-      <c r="CO6" s="2" t="n">
+      <c r="CU6" s="2" t="n">
         <v>0.08877575801176267</v>
       </c>
-      <c r="CP6" s="2" t="n">
+      <c r="CV6" s="2" t="n">
         <v>0.4721934144779466</v>
       </c>
-      <c r="CQ6" s="2" t="n">
+      <c r="CW6" s="2" t="n">
         <v>0.8583581226193799</v>
       </c>
-      <c r="CR6" s="2" t="n">
+      <c r="CX6" s="2" t="n">
         <v>1.288792027011686</v>
       </c>
-      <c r="CS6" s="2" t="inlineStr"/>
-      <c r="CT6" s="2" t="inlineStr"/>
-      <c r="CU6" s="2" t="inlineStr"/>
-      <c r="CV6" s="2" t="inlineStr"/>
-      <c r="CW6" s="2" t="inlineStr"/>
-      <c r="CX6" s="2" t="inlineStr"/>
       <c r="CY6" s="2" t="inlineStr"/>
       <c r="CZ6" s="2" t="inlineStr"/>
-      <c r="DA6" s="2" t="n">
+      <c r="DA6" s="2" t="inlineStr"/>
+      <c r="DB6" s="2" t="inlineStr"/>
+      <c r="DC6" s="2" t="inlineStr"/>
+      <c r="DD6" s="2" t="inlineStr"/>
+      <c r="DE6" s="2" t="inlineStr"/>
+      <c r="DF6" s="2" t="inlineStr"/>
+      <c r="DG6" s="2" t="inlineStr"/>
+      <c r="DH6" s="2" t="inlineStr"/>
+      <c r="DI6" s="2" t="inlineStr"/>
+      <c r="DJ6" s="2" t="inlineStr"/>
+      <c r="DK6" s="2" t="n">
         <v>4670.54264551803</v>
       </c>
-      <c r="DB6" s="2" t="n">
+      <c r="DL6" s="2" t="n">
         <v>8302.095497106837</v>
       </c>
-      <c r="DC6" s="2" t="n">
+      <c r="DM6" s="2" t="n">
+        <v>1356.373827666667</v>
+      </c>
+      <c r="DN6" s="2" t="n">
         <v>21.25577454786666</v>
       </c>
-      <c r="DD6" s="2" t="n">
+      <c r="DO6" s="2" t="n">
         <v>0.06392763143392483</v>
       </c>
-      <c r="DE6" s="2" t="n">
+      <c r="DP6" s="2" t="n">
         <v>0.08966666666666667</v>
       </c>
-      <c r="DF6" s="2" t="n">
+      <c r="DQ6" s="2" t="n">
         <v>0.1076666666666667</v>
       </c>
-      <c r="DG6" s="2" t="n">
+      <c r="DR6" s="2" t="n">
         <v>21.60002667737285</v>
       </c>
-      <c r="DH6" s="2" t="n">
+      <c r="DS6" s="2" t="n">
         <v>35.19727360308286</v>
       </c>
-      <c r="DI6" s="2" t="n">
+      <c r="DT6" s="2" t="n">
         <v>41.52433333333334</v>
       </c>
-      <c r="DJ6" s="2" t="n">
+      <c r="DU6" s="2" t="n">
         <v>59.41233333333334</v>
       </c>
-      <c r="DK6" s="2" t="n">
+      <c r="DV6" s="2" t="n">
         <v>2.206354707253672</v>
       </c>
-      <c r="DL6" s="2" t="n">
+      <c r="DW6" s="2" t="n">
         <v>3.875111753371869</v>
       </c>
-      <c r="DM6" s="2" t="n">
+      <c r="DX6" s="2" t="n">
         <v>5.955</v>
       </c>
-      <c r="DN6" s="2" t="n">
+      <c r="DY6" s="2" t="n">
         <v>18.75633333333333</v>
       </c>
-      <c r="DO6" s="2" t="inlineStr"/>
-      <c r="DP6" s="2" t="inlineStr"/>
-      <c r="DQ6" s="2" t="inlineStr"/>
-      <c r="DR6" s="2" t="inlineStr"/>
-      <c r="DS6" s="2" t="inlineStr"/>
-      <c r="DT6" s="2" t="inlineStr"/>
-      <c r="DU6" s="2" t="inlineStr"/>
-      <c r="DV6" s="2" t="inlineStr"/>
-      <c r="DW6" s="2" t="n">
+      <c r="DZ6" s="2" t="inlineStr"/>
+      <c r="EA6" s="2" t="inlineStr"/>
+      <c r="EB6" s="2" t="inlineStr"/>
+      <c r="EC6" s="2" t="inlineStr"/>
+      <c r="ED6" s="2" t="inlineStr"/>
+      <c r="EE6" s="2" t="inlineStr"/>
+      <c r="EF6" s="2" t="inlineStr"/>
+      <c r="EG6" s="2" t="inlineStr"/>
+      <c r="EH6" s="2" t="inlineStr"/>
+      <c r="EI6" s="2" t="inlineStr"/>
+      <c r="EJ6" s="2" t="inlineStr"/>
+      <c r="EK6" s="2" t="inlineStr"/>
+      <c r="EL6" s="2" t="n">
         <v>0.007878202645421047</v>
       </c>
-      <c r="DX6" s="2" t="n">
+      <c r="EM6" s="2" t="n">
         <v>0.02381365854831143</v>
       </c>
-      <c r="DY6" s="2" t="n">
+      <c r="EN6" s="2" t="n">
+        <v>0.001657523159221254</v>
+      </c>
+      <c r="EO6" s="2" t="n">
         <v>7.637296660300615e-06</v>
       </c>
-      <c r="DZ6" s="2" t="n">
+      <c r="EP6" s="2" t="n">
         <v>5.227066366655701e-05</v>
       </c>
-      <c r="EA6" s="2" t="n">
+      <c r="EQ6" s="2" t="n">
         <v>5.854280947220676e-05</v>
       </c>
-      <c r="EB6" s="2" t="n">
+      <c r="ER6" s="2" t="n">
         <v>4.312194513060097e-05</v>
       </c>
-      <c r="EC6" s="2" t="n">
+      <c r="ES6" s="2" t="n">
         <v>3.092135732415844e-05</v>
       </c>
-      <c r="ED6" s="2" t="n">
+      <c r="ET6" s="2" t="n">
         <v>5.467835108986821e-05</v>
       </c>
-      <c r="EE6" s="2" t="n">
+      <c r="EU6" s="2" t="n">
         <v>5.348853159116194e-05</v>
       </c>
-      <c r="EF6" s="2" t="n">
+      <c r="EV6" s="2" t="n">
         <v>4.025857388762304e-05</v>
       </c>
-      <c r="EG6" s="2" t="n">
+      <c r="EW6" s="2" t="n">
         <v>4.023639432041506e-05</v>
       </c>
-      <c r="EH6" s="2" t="n">
+      <c r="EX6" s="2" t="n">
         <v>0.0001218528508415466</v>
       </c>
-      <c r="EI6" s="2" t="n">
+      <c r="EY6" s="2" t="n">
         <v>0.0001441407426732796</v>
       </c>
-      <c r="EJ6" s="2" t="n">
+      <c r="EZ6" s="2" t="n">
         <v>6.871236526391189e-05</v>
       </c>
-      <c r="EK6" s="2" t="inlineStr"/>
-      <c r="EL6" s="2" t="inlineStr"/>
-      <c r="EM6" s="2" t="inlineStr"/>
-      <c r="EN6" s="2" t="inlineStr"/>
-      <c r="EO6" s="2" t="inlineStr"/>
-      <c r="EP6" s="2" t="inlineStr"/>
-      <c r="EQ6" s="2" t="inlineStr"/>
-      <c r="ER6" s="2" t="inlineStr"/>
-      <c r="ES6" s="2" t="inlineStr">
+      <c r="FA6" s="2" t="inlineStr"/>
+      <c r="FB6" s="2" t="inlineStr"/>
+      <c r="FC6" s="2" t="inlineStr"/>
+      <c r="FD6" s="2" t="inlineStr"/>
+      <c r="FE6" s="2" t="inlineStr"/>
+      <c r="FF6" s="2" t="inlineStr"/>
+      <c r="FG6" s="2" t="inlineStr"/>
+      <c r="FH6" s="2" t="inlineStr"/>
+      <c r="FI6" s="2" t="inlineStr"/>
+      <c r="FJ6" s="2" t="inlineStr"/>
+      <c r="FK6" s="2" t="inlineStr"/>
+      <c r="FL6" s="2" t="inlineStr"/>
+      <c r="FM6" s="2" t="inlineStr">
         <is>
           <t>['dbaas-navigator_ycsb_mysql-scalegrid-aws_0_Hcb2Kigh', 'dbaas-navigator_ycsb_mysql-scalegrid-aws_0_IK9U7vAF', 'dbaas-navigator_ycsb_mysql-scalegrid-aws_0_YSI8P1vQ']</t>
         </is>
       </c>
-      <c r="ET6" s="2" t="n">
+      <c r="FN6" s="2" t="n">
         <v>2828.4</v>
       </c>
-      <c r="EU6" s="2" t="n">
+      <c r="FO6" s="2" t="n">
         <v>2.935262161330376</v>
       </c>
-      <c r="EV6" s="2" t="n">
+      <c r="FP6" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="EW6" s="2" t="n">
+      <c r="FQ6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EX6" s="2" t="n">
+      <c r="FR6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="EY6" s="2" t="n">
+      <c r="FS6" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="EZ6" s="2" t="n">
+      <c r="FT6" s="2" t="n">
         <v>-1</v>
       </c>
-      <c r="FA6" s="3" t="n">
+      <c r="FU6" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FV6" s="3" t="n">
         <v>14</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>benchANT</t>
+        </is>
+      </c>
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>dbaas-navigator</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>ycsb</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>planetscale-aws</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>planetscale-aws</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>EC2</t>
+        </is>
+      </c>
+      <c r="G7" s="2" t="inlineStr">
+        <is>
+          <t>EC2</t>
+        </is>
+      </c>
+      <c r="H7" s="2" t="inlineStr">
+        <is>
+          <t>PLANETSCALE</t>
+        </is>
+      </c>
+      <c r="I7" s="2" t="inlineStr">
+        <is>
+          <t>PLANETSCALE</t>
+        </is>
+      </c>
+      <c r="J7" s="2" t="inlineStr">
+        <is>
+          <t>MYSQL</t>
+        </is>
+      </c>
+      <c r="K7" s="2" t="inlineStr">
+        <is>
+          <t>DBAAS</t>
+        </is>
+      </c>
+      <c r="L7" s="2" t="inlineStr">
+        <is>
+          <t>8.0.21</t>
+        </is>
+      </c>
+      <c r="M7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="N7" s="2" t="n">
+        <v>3484</v>
+      </c>
+      <c r="O7" s="2" t="inlineStr"/>
+      <c r="P7" s="2" t="inlineStr"/>
+      <c r="Q7" s="2" t="inlineStr"/>
+      <c r="R7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="S7" s="2" t="inlineStr"/>
+      <c r="T7" s="2" t="inlineStr"/>
+      <c r="U7" s="2" t="inlineStr"/>
+      <c r="V7" s="2" t="inlineStr"/>
+      <c r="W7" s="2" t="inlineStr"/>
+      <c r="X7" s="2" t="inlineStr"/>
+      <c r="Y7" s="2" t="inlineStr"/>
+      <c r="Z7" s="2" t="inlineStr"/>
+      <c r="AA7" s="2" t="inlineStr">
+        <is>
+          <t>YCSB-Read-Write-Mix</t>
+        </is>
+      </c>
+      <c r="AB7" s="2" t="inlineStr">
+        <is>
+          <t>YCSB</t>
+        </is>
+      </c>
+      <c r="AC7" s="2" t="inlineStr">
+        <is>
+          <t>0.17.0</t>
+        </is>
+      </c>
+      <c r="AD7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AE7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AF7" s="2" t="inlineStr">
+        <is>
+          <t>[]</t>
+        </is>
+      </c>
+      <c r="AG7" s="2" t="inlineStr">
+        <is>
+          <t>LOAD</t>
+        </is>
+      </c>
+      <c r="AH7" s="2" t="inlineStr">
+        <is>
+          <t>site.ycsb.workloads.CoreWorkload</t>
+        </is>
+      </c>
+      <c r="AI7" s="2" t="n">
+        <v>1800</v>
+      </c>
+      <c r="AJ7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="AK7" s="2" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="AL7" s="2" t="n">
+        <v>10000000</v>
+      </c>
+      <c r="AM7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="2" t="n">
+        <v>54000000</v>
+      </c>
+      <c r="AO7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="AQ7" s="2" t="n">
+        <v>500</v>
+      </c>
+      <c r="AR7" s="2" t="b">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="2" t="inlineStr">
+        <is>
+          <t>ZIPFIAN</t>
+        </is>
+      </c>
+      <c r="AU7" s="2" t="inlineStr">
+        <is>
+          <t>UNIFORM</t>
+        </is>
+      </c>
+      <c r="AV7" s="2" t="inlineStr">
+        <is>
+          <t>ORDERED</t>
+        </is>
+      </c>
+      <c r="AW7" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AX7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="2" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="AZ7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="BC7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="BD7" s="2" t="inlineStr"/>
+      <c r="BE7" s="2" t="inlineStr"/>
+      <c r="BF7" s="2" t="inlineStr"/>
+      <c r="BG7" s="2" t="inlineStr"/>
+      <c r="BH7" s="2" t="inlineStr"/>
+      <c r="BI7" s="2" t="inlineStr"/>
+      <c r="BJ7" s="2" t="inlineStr"/>
+      <c r="BK7" s="2" t="inlineStr">
+        <is>
+          <t>us-west-2</t>
+        </is>
+      </c>
+      <c r="BL7" s="2" t="inlineStr">
+        <is>
+          <t>c5.4xlarge</t>
+        </is>
+      </c>
+      <c r="BM7" s="2" t="inlineStr">
+        <is>
+          <t>x86_64</t>
+        </is>
+      </c>
+      <c r="BN7" s="2" t="inlineStr">
+        <is>
+          <t>ubuntu</t>
+        </is>
+      </c>
+      <c r="BO7" s="2" t="n">
+        <v>20.04</v>
+      </c>
+      <c r="BP7" s="2" t="inlineStr">
+        <is>
+          <t>GP2</t>
+        </is>
+      </c>
+      <c r="BQ7" s="2" t="n">
+        <v>30</v>
+      </c>
+      <c r="BR7" s="2" t="n">
+        <v>100</v>
+      </c>
+      <c r="BS7" s="2" t="inlineStr"/>
+      <c r="BT7" s="2" t="inlineStr"/>
+      <c r="BU7" s="2" t="inlineStr"/>
+      <c r="BV7" s="2" t="inlineStr"/>
+      <c r="BW7" s="2" t="inlineStr"/>
+      <c r="BX7" s="2" t="inlineStr"/>
+      <c r="BY7" s="2" t="inlineStr"/>
+      <c r="BZ7" s="2" t="inlineStr"/>
+      <c r="CA7" s="2" t="inlineStr"/>
+      <c r="CB7" s="2" t="inlineStr"/>
+      <c r="CC7" s="2" t="inlineStr"/>
+      <c r="CD7" s="2" t="inlineStr">
+        <is>
+          <t>us-west</t>
+        </is>
+      </c>
+      <c r="CE7" s="2" t="inlineStr">
+        <is>
+          <t>scaler_pro</t>
+        </is>
+      </c>
+      <c r="CF7" s="2" t="inlineStr">
+        <is>
+          <t>PS_640</t>
+        </is>
+      </c>
+      <c r="CG7" s="2" t="n">
+        <v>10</v>
+      </c>
+      <c r="CH7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="CI7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="CJ7" s="2" t="n">
+        <v>50.27294278227787</v>
+      </c>
+      <c r="CK7" s="2" t="n">
+        <v>117.1670324989481</v>
+      </c>
+      <c r="CL7" s="2" t="n">
+        <v>0.2681384972522113</v>
+      </c>
+      <c r="CM7" s="2" t="n">
+        <v>0.4258518579199774</v>
+      </c>
+      <c r="CN7" s="2" t="n">
+        <v>1.696409920757156</v>
+      </c>
+      <c r="CO7" s="2" t="n">
+        <v>3.799010865416887</v>
+      </c>
+      <c r="CP7" s="2" t="n">
+        <v>4.858757408592816</v>
+      </c>
+      <c r="CQ7" s="2" t="n">
+        <v>0.4427548797739387</v>
+      </c>
+      <c r="CR7" s="2" t="n">
+        <v>0.873052105777832</v>
+      </c>
+      <c r="CS7" s="2" t="n">
+        <v>0.9800571411912675</v>
+      </c>
+      <c r="CT7" s="2" t="n">
+        <v>1.268212390203891</v>
+      </c>
+      <c r="CU7" s="2" t="n">
+        <v>0.2980994816390759</v>
+      </c>
+      <c r="CV7" s="2" t="n">
+        <v>0.6267844813019399</v>
+      </c>
+      <c r="CW7" s="2" t="n">
+        <v>1.304286267146391</v>
+      </c>
+      <c r="CX7" s="2" t="n">
+        <v>1.701926751263598</v>
+      </c>
+      <c r="CY7" s="2" t="inlineStr"/>
+      <c r="CZ7" s="2" t="inlineStr"/>
+      <c r="DA7" s="2" t="inlineStr"/>
+      <c r="DB7" s="2" t="inlineStr"/>
+      <c r="DC7" s="2" t="inlineStr"/>
+      <c r="DD7" s="2" t="inlineStr"/>
+      <c r="DE7" s="2" t="inlineStr"/>
+      <c r="DF7" s="2" t="inlineStr"/>
+      <c r="DG7" s="2" t="inlineStr"/>
+      <c r="DH7" s="2" t="inlineStr"/>
+      <c r="DI7" s="2" t="inlineStr"/>
+      <c r="DJ7" s="2" t="inlineStr"/>
+      <c r="DK7" s="2" t="n">
+        <v>3617.46417177617</v>
+      </c>
+      <c r="DL7" s="2" t="n">
+        <v>5677.894799655413</v>
+      </c>
+      <c r="DM7" s="2" t="n">
+        <v>308.628335</v>
+      </c>
+      <c r="DN7" s="2" t="n">
+        <v>27.45614939396667</v>
+      </c>
+      <c r="DO7" s="2" t="n">
+        <v>36.60949795164839</v>
+      </c>
+      <c r="DP7" s="2" t="n">
+        <v>271.5296666666667</v>
+      </c>
+      <c r="DQ7" s="2" t="n">
+        <v>311.4656666666667</v>
+      </c>
+      <c r="DR7" s="2" t="n">
+        <v>27.1368239398343</v>
+      </c>
+      <c r="DS7" s="2" t="n">
+        <v>42.45313487475916</v>
+      </c>
+      <c r="DT7" s="2" t="n">
+        <v>49.631</v>
+      </c>
+      <c r="DU7" s="2" t="n">
+        <v>63.071</v>
+      </c>
+      <c r="DV7" s="2" t="n">
+        <v>7.668659626450143</v>
+      </c>
+      <c r="DW7" s="2" t="n">
+        <v>12.70500385356454</v>
+      </c>
+      <c r="DX7" s="2" t="n">
+        <v>17.399</v>
+      </c>
+      <c r="DY7" s="2" t="n">
+        <v>30.751</v>
+      </c>
+      <c r="DZ7" s="2" t="inlineStr"/>
+      <c r="EA7" s="2" t="inlineStr"/>
+      <c r="EB7" s="2" t="inlineStr"/>
+      <c r="EC7" s="2" t="inlineStr"/>
+      <c r="ED7" s="2" t="inlineStr"/>
+      <c r="EE7" s="2" t="inlineStr"/>
+      <c r="EF7" s="2" t="inlineStr"/>
+      <c r="EG7" s="2" t="inlineStr"/>
+      <c r="EH7" s="2" t="inlineStr"/>
+      <c r="EI7" s="2" t="inlineStr"/>
+      <c r="EJ7" s="2" t="inlineStr"/>
+      <c r="EK7" s="2" t="inlineStr"/>
+      <c r="EL7" s="2" t="n">
+        <v>0.01389728837524158</v>
+      </c>
+      <c r="EM7" s="2" t="n">
+        <v>0.02063564694894644</v>
+      </c>
+      <c r="EN7" s="2" t="n">
+        <v>0.0008688071276806498</v>
+      </c>
+      <c r="EO7" s="2" t="n">
+        <v>1.551025425340801e-05</v>
+      </c>
+      <c r="EP7" s="2" t="n">
+        <v>4.633797281234699e-05</v>
+      </c>
+      <c r="EQ7" s="2" t="n">
+        <v>1.399114473219091e-05</v>
+      </c>
+      <c r="ER7" s="2" t="n">
+        <v>1.559965649052645e-05</v>
+      </c>
+      <c r="ES7" s="2" t="n">
+        <v>1.631564846186795e-05</v>
+      </c>
+      <c r="ET7" s="2" t="n">
+        <v>2.056507978394104e-05</v>
+      </c>
+      <c r="EU7" s="2" t="n">
+        <v>1.974687475955084e-05</v>
+      </c>
+      <c r="EV7" s="2" t="n">
+        <v>2.010769434770166e-05</v>
+      </c>
+      <c r="EW7" s="2" t="n">
+        <v>3.887243614397677e-05</v>
+      </c>
+      <c r="EX7" s="2" t="n">
+        <v>4.933367108944935e-05</v>
+      </c>
+      <c r="EY7" s="2" t="n">
+        <v>7.496328910548829e-05</v>
+      </c>
+      <c r="EZ7" s="2" t="n">
+        <v>5.53454115724236e-05</v>
+      </c>
+      <c r="FA7" s="2" t="inlineStr"/>
+      <c r="FB7" s="2" t="inlineStr"/>
+      <c r="FC7" s="2" t="inlineStr"/>
+      <c r="FD7" s="2" t="inlineStr"/>
+      <c r="FE7" s="2" t="inlineStr"/>
+      <c r="FF7" s="2" t="inlineStr"/>
+      <c r="FG7" s="2" t="inlineStr"/>
+      <c r="FH7" s="2" t="inlineStr"/>
+      <c r="FI7" s="2" t="inlineStr"/>
+      <c r="FJ7" s="2" t="inlineStr"/>
+      <c r="FK7" s="2" t="inlineStr"/>
+      <c r="FL7" s="2" t="inlineStr"/>
+      <c r="FM7" s="2" t="inlineStr">
+        <is>
+          <t>['dbaas-navigator_ycsb_planetscale-aws_0_6mcsVx4A', 'dbaas-navigator_ycsb_planetscale-aws_0_IWksNUf1', 'dbaas-navigator_ycsb_planetscale-aws_0_KMIYSQdj']</t>
+        </is>
+      </c>
+      <c r="FN7" s="2" t="n">
+        <v>3484</v>
+      </c>
+      <c r="FO7" s="2" t="n">
+        <v>1.629705740429223</v>
+      </c>
+      <c r="FP7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FQ7" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="FR7" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="FS7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="FT7" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FU7" s="2" t="n">
+        <v>-1</v>
+      </c>
+      <c r="FV7" s="3" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>